<commit_message>
Added InterfacEnd FQN column to excel export - (Task #739)
---
Task #739: Give user way to directly get FQN of InterfaceEnds in Excel
Export
</commit_message>
<xml_diff>
--- a/de.dlr.sc.virsat.model.extension.funcelectrical.test/resources/SampleTest.xlsx
+++ b/de.dlr.sc.virsat.model.extension.funcelectrical.test/resources/SampleTest.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20366"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muel_s8\git\VirtualSatellite4-Core\de.dlr.sc.virsat.model.extension.funcelectrical.test\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70991D57-1655-49F9-90C1-4EA677B81FFC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="105" windowWidth="20115" windowHeight="9525" activeTab="3"/>
+    <workbookView xWindow="600" yWindow="105" windowWidth="20115" windowHeight="9525" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Header" sheetId="1" r:id="rId1"/>
@@ -17,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
   <si>
     <t xml:space="preserve"> Structural Element UUID</t>
   </si>
@@ -92,12 +98,15 @@
   </si>
   <si>
     <t>VirSat IO Sheet for Interfaces</t>
+  </si>
+  <si>
+    <t>InterfaceEnd FullQualifiedName</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -349,7 +358,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -380,6 +389,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -411,14 +423,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -456,9 +471,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -491,9 +506,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -526,9 +558,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -701,7 +750,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -716,25 +765,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20"/>
-      <c r="B1" s="20"/>
+      <c r="A1" s="21"/>
+      <c r="B1" s="21"/>
       <c r="C1" s="14"/>
     </row>
     <row r="2" spans="1:3" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
     </row>
     <row r="3" spans="1:3" ht="128.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="23"/>
+      <c r="C3" s="24"/>
     </row>
     <row r="4" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
@@ -817,11 +866,11 @@
       <c r="C15" s="6"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="21" t="s">
+      <c r="A37" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="B37" s="21"/>
-      <c r="C37" s="21"/>
+      <c r="B37" s="22"/>
+      <c r="C37" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -836,7 +885,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -851,25 +900,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20"/>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
+      <c r="A1" s="21"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
     </row>
     <row r="2" spans="1:3" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
     </row>
     <row r="3" spans="1:3" ht="128.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="20"/>
+      <c r="C3" s="21"/>
     </row>
     <row r="4" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
@@ -888,9 +937,9 @@
       <c r="C5" s="9"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="25"/>
-      <c r="B37" s="26"/>
-      <c r="C37" s="26"/>
+      <c r="A37" s="26"/>
+      <c r="B37" s="27"/>
+      <c r="C37" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -905,46 +954,49 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.5703125" style="3" customWidth="1"/>
     <col min="2" max="2" width="8.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" style="2" customWidth="1"/>
+    <col min="3" max="4" width="26.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="33.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20"/>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-    </row>
-    <row r="2" spans="1:4" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24" t="s">
+    <row r="1" spans="1:5" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="21"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+    </row>
+    <row r="2" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-    </row>
-    <row r="3" spans="1:4" ht="128.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+    </row>
+    <row r="3" spans="1:5" ht="128.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-    </row>
-    <row r="4" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+    </row>
+    <row r="4" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>15</v>
       </c>
@@ -957,23 +1009,28 @@
       <c r="D4" s="17" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="E4" s="17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
-      <c r="D5" s="9"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="25"/>
-      <c r="B37" s="26"/>
-      <c r="C37" s="26"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="9"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="26"/>
+      <c r="B37" s="27"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="B3:E3"/>
     <mergeCell ref="A37:C37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -982,10 +1039,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
@@ -999,31 +1056,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20"/>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
+      <c r="A1" s="21"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
     </row>
     <row r="2" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
     </row>
     <row r="3" spans="1:5" ht="128.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
     </row>
     <row r="4" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
@@ -1050,9 +1107,9 @@
       <c r="E5" s="9"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="25"/>
-      <c r="B37" s="26"/>
-      <c r="C37" s="26"/>
+      <c r="A37" s="26"/>
+      <c r="B37" s="27"/>
+      <c r="C37" s="27"/>
       <c r="D37" s="19"/>
     </row>
   </sheetData>

</xml_diff>